<commit_message>
FANG, SIMO, AMZN, OXY
</commit_message>
<xml_diff>
--- a/AMZN.xlsx
+++ b/AMZN.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Desktop\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C54BAD0-3017-4957-ADAC-847E5359B4B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00E3D59E-75A2-4A9D-88EE-5E2558434F5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{319C79D3-530A-422D-B7D4-1569BBD88715}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{319C79D3-530A-422D-B7D4-1569BBD88715}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -853,7 +853,7 @@
   <dimension ref="J2:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -866,7 +866,7 @@
         <v>1</v>
       </c>
       <c r="K2" s="1">
-        <v>140.80000000000001</v>
+        <v>142.1</v>
       </c>
       <c r="L2" s="21">
         <v>44779</v>
@@ -889,7 +889,7 @@
       </c>
       <c r="K4" s="2">
         <f>K3*K2</f>
-        <v>1434470.4000000001</v>
+        <v>1447714.8</v>
       </c>
       <c r="L4" s="3"/>
     </row>
@@ -922,7 +922,7 @@
       </c>
       <c r="K7" s="2">
         <f>K4-K5+K6</f>
-        <v>1440284.4000000001</v>
+        <v>1453528.8</v>
       </c>
       <c r="L7" s="3"/>
     </row>
@@ -948,10 +948,10 @@
   <dimension ref="A1:DN66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="AQ4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="AQ19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="BA30" sqref="BA30"/>
+      <selection pane="bottomRight" activeCell="BG46" sqref="BG46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>